<commit_message>
Fix trailing space on PETase ancestor part
</commit_message>
<xml_diff>
--- a/Plastic Degradation/Plastic Degradation.xlsx
+++ b/Plastic Degradation/Plastic Degradation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Plastic Degradation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED017F7-FA77-9E4E-BA60-A500A223CD50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846BA00A-1C0C-FA48-92CA-9213CD191A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25620" yWindow="-2320" windowWidth="25620" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25620" yWindow="-2320" windowWidth="25620" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -22797,10 +22797,10 @@
     <t>IsPETase-ML_Mu_1</t>
   </si>
   <si>
-    <t>PETase-WT, PETase-EcCO-WT, PETase-S238F_W159H, PETase-K2010999, PETase-T88A_S93M_S121E_W159F_D186H_R280A, PETase-S121E_D186H_R280A, PETase_Reconstructed_Ancestor_1 , IsPETase-W159H-S238F, IsPETase-ML_Mu_1, IsPETase-T88F-I208Y-S238F-S245Y-R280A</t>
-  </si>
-  <si>
     <t>BHETase_1, BHETase_2</t>
+  </si>
+  <si>
+    <t>PETase-WT, PETase-EcCO-WT, PETase-S238F_W159H, PETase-K2010999, PETase-T88A_S93M_S121E_W159F_D186H_R280A, PETase-S121E_D186H_R280A, PETase_Reconstructed_Ancestor_1, IsPETase-W159H-S238F, IsPETase-ML_Mu_1, IsPETase-T88F-I208Y-S238F-S245Y-R280A</t>
   </si>
 </sst>
 </file>
@@ -23194,15 +23194,15 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -23659,7 +23659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -23734,14 +23734,14 @@
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:13" ht="46" customHeight="1">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="53" t="s">
         <v>7555</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="51"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="55"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -23986,7 +23986,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A15" s="55" t="s">
+      <c r="A15" s="52" t="s">
         <v>7544</v>
       </c>
       <c r="B15" s="41" t="s">
@@ -24000,7 +24000,7 @@
       <c r="F15" s="18" t="s">
         <v>7521</v>
       </c>
-      <c r="G15" s="53"/>
+      <c r="G15" s="50"/>
       <c r="H15" s="41" t="s">
         <v>7547</v>
       </c>
@@ -24020,7 +24020,7 @@
       <c r="M15" s="19"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A16" s="55" t="s">
+      <c r="A16" s="52" t="s">
         <v>7554</v>
       </c>
       <c r="B16" s="41" t="s">
@@ -24034,7 +24034,7 @@
       <c r="F16" s="18" t="s">
         <v>7521</v>
       </c>
-      <c r="G16" s="53"/>
+      <c r="G16" s="50"/>
       <c r="H16" s="18" t="s">
         <v>7417</v>
       </c>
@@ -24054,7 +24054,7 @@
       <c r="M16" s="41"/>
     </row>
     <row r="17" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A17" s="55" t="s">
+      <c r="A17" s="52" t="s">
         <v>7545</v>
       </c>
       <c r="B17" s="41" t="s">
@@ -24068,7 +24068,7 @@
       <c r="F17" s="18" t="s">
         <v>7521</v>
       </c>
-      <c r="G17" s="53"/>
+      <c r="G17" s="50"/>
       <c r="H17" s="18" t="s">
         <v>7417</v>
       </c>
@@ -24088,7 +24088,7 @@
       <c r="M17" s="22"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A18" s="55" t="s">
+      <c r="A18" s="52" t="s">
         <v>7546</v>
       </c>
       <c r="B18" s="41" t="s">
@@ -24102,7 +24102,7 @@
       <c r="F18" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G18" s="53" t="s">
+      <c r="G18" s="50" t="s">
         <v>7543</v>
       </c>
       <c r="H18" s="18" t="s">
@@ -24138,7 +24138,7 @@
       <c r="F19" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G19" s="54" t="s">
+      <c r="G19" s="51" t="s">
         <v>7532</v>
       </c>
       <c r="H19" s="18" t="s">
@@ -24174,7 +24174,7 @@
       <c r="F20" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G20" s="54" t="s">
+      <c r="G20" s="51" t="s">
         <v>7533</v>
       </c>
       <c r="H20" s="18" t="s">
@@ -24210,7 +24210,7 @@
       <c r="F21" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="54" t="s">
+      <c r="G21" s="51" t="s">
         <v>7534</v>
       </c>
       <c r="H21" s="18" t="s">
@@ -24246,7 +24246,7 @@
       <c r="F22" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G22" s="54" t="s">
+      <c r="G22" s="51" t="s">
         <v>7535</v>
       </c>
       <c r="H22" s="18" t="s">
@@ -24282,7 +24282,7 @@
       <c r="F23" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G23" s="54" t="s">
+      <c r="G23" s="51" t="s">
         <v>7536</v>
       </c>
       <c r="H23" s="18" t="s">
@@ -24318,7 +24318,7 @@
       <c r="F24" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G24" s="54" t="s">
+      <c r="G24" s="51" t="s">
         <v>7538</v>
       </c>
       <c r="H24" s="18" t="s">
@@ -24354,7 +24354,7 @@
       <c r="F25" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G25" s="54" t="s">
+      <c r="G25" s="51" t="s">
         <v>7539</v>
       </c>
       <c r="H25" s="18" t="s">
@@ -24390,7 +24390,7 @@
       <c r="F26" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G26" s="54" t="s">
+      <c r="G26" s="51" t="s">
         <v>7540</v>
       </c>
       <c r="H26" s="18" t="s">
@@ -24424,7 +24424,7 @@
       <c r="F27" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G27" s="54" t="s">
+      <c r="G27" s="51" t="s">
         <v>7501</v>
       </c>
       <c r="H27" s="18" t="s">
@@ -24467,7 +24467,7 @@
       <c r="D29" s="20"/>
       <c r="E29" s="18"/>
       <c r="F29" s="18"/>
-      <c r="G29" s="54"/>
+      <c r="G29" s="51"/>
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
       <c r="J29" s="18" t="b">
@@ -24489,7 +24489,7 @@
       <c r="D30" s="20"/>
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
-      <c r="G30" s="54"/>
+      <c r="G30" s="51"/>
       <c r="H30" s="18"/>
       <c r="I30" s="18"/>
       <c r="J30" s="18" t="b">
@@ -24511,7 +24511,7 @@
       <c r="D31" s="20"/>
       <c r="E31" s="18"/>
       <c r="F31" s="18"/>
-      <c r="G31" s="54"/>
+      <c r="G31" s="51"/>
       <c r="H31" s="18"/>
       <c r="I31" s="18"/>
       <c r="J31" s="18" t="b">
@@ -24533,7 +24533,7 @@
       <c r="D32" s="20"/>
       <c r="E32" s="18"/>
       <c r="F32" s="18"/>
-      <c r="G32" s="54"/>
+      <c r="G32" s="51"/>
       <c r="H32" s="18"/>
       <c r="I32" s="18"/>
       <c r="J32" s="18" t="b">
@@ -24555,7 +24555,7 @@
       <c r="D33" s="20"/>
       <c r="E33" s="18"/>
       <c r="F33" s="18"/>
-      <c r="G33" s="54"/>
+      <c r="G33" s="51"/>
       <c r="H33" s="18"/>
       <c r="I33" s="18"/>
       <c r="J33" s="18" t="b">
@@ -24577,7 +24577,7 @@
       <c r="D34" s="20"/>
       <c r="E34" s="18"/>
       <c r="F34" s="18"/>
-      <c r="G34" s="54"/>
+      <c r="G34" s="51"/>
       <c r="H34" s="18"/>
       <c r="I34" s="18"/>
       <c r="J34" s="18" t="b">
@@ -24599,7 +24599,7 @@
       <c r="D35" s="20"/>
       <c r="E35" s="18"/>
       <c r="F35" s="18"/>
-      <c r="G35" s="54"/>
+      <c r="G35" s="51"/>
       <c r="H35" s="18"/>
       <c r="I35" s="18"/>
       <c r="J35" s="18" t="b">
@@ -25677,8 +25677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -26171,7 +26171,7 @@
       <c r="X13" s="3"/>
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1">
-      <c r="A14" s="55" t="s">
+      <c r="A14" s="52" t="s">
         <v>7556</v>
       </c>
       <c r="B14" s="21"/>
@@ -26182,8 +26182,8 @@
         <v>7501</v>
       </c>
       <c r="F14" s="18"/>
-      <c r="G14" s="55" t="s">
-        <v>7564</v>
+      <c r="G14" s="52" t="s">
+        <v>7565</v>
       </c>
       <c r="H14" s="18"/>
       <c r="I14" s="32"/>
@@ -26204,7 +26204,7 @@
       <c r="X14" s="3"/>
     </row>
     <row r="15" spans="1:26" ht="16">
-      <c r="A15" s="55" t="s">
+      <c r="A15" s="52" t="s">
         <v>7557</v>
       </c>
       <c r="B15" s="21"/>
@@ -26217,7 +26217,7 @@
       </c>
       <c r="F15" s="18"/>
       <c r="G15" s="41" t="s">
-        <v>7565</v>
+        <v>7564</v>
       </c>
       <c r="H15" s="21"/>
       <c r="I15" s="18"/>
@@ -69366,7 +69366,7 @@
       <c r="C29" s="3"/>
     </row>
     <row r="30" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A30" s="52" t="s">
+      <c r="A30" s="49" t="s">
         <v>7547</v>
       </c>
       <c r="B30" s="18">

</xml_diff>

<commit_message>
remove unexpected whitespace from end of "PETase_Reconstructed_Ancestor_1" File https://github.com/SynBioDex/SBOL-utilities/issues/37 to be more tolerant of whitespace issues
</commit_message>
<xml_diff>
--- a/Plastic Degradation/Plastic Degradation.xlsx
+++ b/Plastic Degradation/Plastic Degradation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinoo/_dev/distribution/iGEM-distribution/Plastic Degradation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakebeal/projects/BioTools/iGEM_distribution/Plastic Degradation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846BA00A-1C0C-FA48-92CA-9213CD191A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBF5623-9C8B-1E43-BCAC-011BF1FB5391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25620" yWindow="-2320" windowWidth="25620" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts and Devices" sheetId="1" r:id="rId1"/>
@@ -29,9 +29,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -22791,9 +22789,6 @@
     <t>BHETase_2</t>
   </si>
   <si>
-    <t xml:space="preserve">PETase_Reconstructed_Ancestor_1 </t>
-  </si>
-  <si>
     <t>IsPETase-ML_Mu_1</t>
   </si>
   <si>
@@ -22801,6 +22796,9 @@
   </si>
   <si>
     <t>PETase-WT, PETase-EcCO-WT, PETase-S238F_W159H, PETase-K2010999, PETase-T88A_S93M_S121E_W159F_D186H_R280A, PETase-S121E_D186H_R280A, PETase_Reconstructed_Ancestor_1, IsPETase-W159H-S238F, IsPETase-ML_Mu_1, IsPETase-T88F-I208Y-S238F-S245Y-R280A</t>
+  </si>
+  <si>
+    <t>PETase_Reconstructed_Ancestor_1</t>
   </si>
 </sst>
 </file>
@@ -23659,8 +23657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M983"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -24269,7 +24267,7 @@
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1">
       <c r="A23" s="41" t="s">
-        <v>7562</v>
+        <v>7565</v>
       </c>
       <c r="B23" s="41" t="s">
         <v>47</v>
@@ -24341,7 +24339,7 @@
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1">
       <c r="A25" s="41" t="s">
-        <v>7563</v>
+        <v>7562</v>
       </c>
       <c r="B25" s="41" t="s">
         <v>47</v>
@@ -25677,8 +25675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -26183,7 +26181,7 @@
       </c>
       <c r="F14" s="18"/>
       <c r="G14" s="52" t="s">
-        <v>7565</v>
+        <v>7564</v>
       </c>
       <c r="H14" s="18"/>
       <c r="I14" s="32"/>
@@ -26217,7 +26215,7 @@
       </c>
       <c r="F15" s="18"/>
       <c r="G15" s="41" t="s">
-        <v>7564</v>
+        <v>7563</v>
       </c>
       <c r="H15" s="21"/>
       <c r="I15" s="18"/>

</xml_diff>